<commit_message>
parse amendments and misc formatting ixes
</commit_message>
<xml_diff>
--- a/src/integration_mapping_dict.xlsx
+++ b/src/integration_mapping_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bullenca/Work/Repos/ChildhoodCancerDataInitiative-MCI_JSON2TSV/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3578ACB-D51C-B346-BD77-1FD671CE1ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106366DA-A8AF-6E4E-A5BB-D1847406A42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="940" windowWidth="29760" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="integration_mapping_dict" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">integration_mapping_dict!$A$1:$H$858</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">integration_mapping_dict!$A$1:$H$866</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4301" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4320" uniqueCount="1115">
   <si>
     <t>type</t>
   </si>
@@ -3359,6 +3359,15 @@
   </si>
   <si>
     <t>Pertinent Genes with No Observed Relevant Alterations</t>
+  </si>
+  <si>
+    <t>amendments</t>
+  </si>
+  <si>
+    <t>WXS Report Amendments</t>
+  </si>
+  <si>
+    <t>Fusion Report Amendments</t>
   </si>
 </sst>
 </file>
@@ -3748,10 +3757,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H860"/>
+  <dimension ref="A1:H866"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C834" workbookViewId="0">
-      <selection activeCell="D865" sqref="D865"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19585,13 +19594,10 @@
         <v>1015</v>
       </c>
       <c r="C789" t="s">
-        <v>1019</v>
+        <v>1112</v>
       </c>
       <c r="D789" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E789" t="s">
-        <v>86</v>
+        <v>1113</v>
       </c>
       <c r="G789" s="3">
         <v>5</v>
@@ -19605,10 +19611,10 @@
         <v>1015</v>
       </c>
       <c r="C790" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="D790" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="E790" t="s">
         <v>86</v>
@@ -19625,10 +19631,10 @@
         <v>1015</v>
       </c>
       <c r="C791" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D791" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="E791" t="s">
         <v>86</v>
@@ -19645,10 +19651,10 @@
         <v>1015</v>
       </c>
       <c r="C792" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D792" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="E792" t="s">
         <v>86</v>
@@ -19665,10 +19671,10 @@
         <v>1015</v>
       </c>
       <c r="C793" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D793" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="E793" t="s">
         <v>86</v>
@@ -19682,16 +19688,19 @@
         <v>1014</v>
       </c>
       <c r="B794" t="s">
-        <v>1029</v>
+        <v>1015</v>
       </c>
       <c r="C794" t="s">
-        <v>1001</v>
+        <v>1027</v>
       </c>
       <c r="D794" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E794" t="s">
+        <v>86</v>
+      </c>
+      <c r="G794" s="3">
         <v>10</v>
-      </c>
-      <c r="G794" s="3">
-        <v>1</v>
       </c>
     </row>
     <row r="795" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19702,13 +19711,13 @@
         <v>1029</v>
       </c>
       <c r="C795" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D795" t="s">
-        <v>1016</v>
+        <v>10</v>
       </c>
       <c r="G795" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="796" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19719,13 +19728,13 @@
         <v>1029</v>
       </c>
       <c r="C796" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D796" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="G796" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="797" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19736,13 +19745,13 @@
         <v>1029</v>
       </c>
       <c r="C797" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D797" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="G797" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="798" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19753,16 +19762,13 @@
         <v>1029</v>
       </c>
       <c r="C798" t="s">
-        <v>1108</v>
+        <v>1006</v>
       </c>
       <c r="D798" t="s">
-        <v>1091</v>
-      </c>
-      <c r="E798" t="s">
-        <v>86</v>
+        <v>1018</v>
       </c>
       <c r="G798" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="799" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19773,16 +19779,13 @@
         <v>1029</v>
       </c>
       <c r="C799" t="s">
-        <v>1030</v>
+        <v>1112</v>
       </c>
       <c r="D799" t="s">
-        <v>1031</v>
-      </c>
-      <c r="E799" t="s">
-        <v>86</v>
+        <v>1113</v>
       </c>
       <c r="G799" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="800" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19793,16 +19796,16 @@
         <v>1029</v>
       </c>
       <c r="C800" t="s">
-        <v>1027</v>
+        <v>1108</v>
       </c>
       <c r="D800" t="s">
-        <v>1032</v>
+        <v>1091</v>
       </c>
       <c r="E800" t="s">
         <v>86</v>
       </c>
       <c r="G800" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="801" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19813,16 +19816,16 @@
         <v>1029</v>
       </c>
       <c r="C801" t="s">
-        <v>1025</v>
+        <v>1030</v>
       </c>
       <c r="D801" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="E801" t="s">
         <v>86</v>
       </c>
       <c r="G801" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="802" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19830,19 +19833,22 @@
         <v>1014</v>
       </c>
       <c r="B802" t="s">
-        <v>1034</v>
+        <v>1029</v>
       </c>
       <c r="C802" t="s">
-        <v>1001</v>
+        <v>1027</v>
       </c>
       <c r="D802" t="s">
-        <v>10</v>
+        <v>1032</v>
+      </c>
+      <c r="E802" t="s">
+        <v>86</v>
       </c>
       <c r="G802" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="803" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="803" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A803" t="s">
         <v>1014</v>
       </c>
@@ -19850,36 +19856,33 @@
         <v>1029</v>
       </c>
       <c r="C803" t="s">
-        <v>1093</v>
+        <v>1025</v>
       </c>
       <c r="D803" t="s">
-        <v>1098</v>
+        <v>1033</v>
       </c>
       <c r="E803" t="s">
         <v>86</v>
       </c>
-      <c r="G803" s="2">
+      <c r="G803" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="804" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="804" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A804" t="s">
         <v>1014</v>
       </c>
       <c r="B804" t="s">
-        <v>1029</v>
+        <v>1034</v>
       </c>
       <c r="C804" t="s">
-        <v>1094</v>
+        <v>1001</v>
       </c>
       <c r="D804" t="s">
-        <v>1099</v>
-      </c>
-      <c r="E804" t="s">
-        <v>86</v>
-      </c>
-      <c r="G804" s="2">
         <v>10</v>
+      </c>
+      <c r="G804" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="805" spans="1:7" x14ac:dyDescent="0.2">
@@ -19890,16 +19893,16 @@
         <v>1029</v>
       </c>
       <c r="C805" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="D805" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="E805" t="s">
         <v>86</v>
       </c>
       <c r="G805" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="806" spans="1:7" x14ac:dyDescent="0.2">
@@ -19910,16 +19913,16 @@
         <v>1029</v>
       </c>
       <c r="C806" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="D806" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="E806" t="s">
         <v>86</v>
       </c>
       <c r="G806" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="807" spans="1:7" x14ac:dyDescent="0.2">
@@ -19930,58 +19933,64 @@
         <v>1029</v>
       </c>
       <c r="C807" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="D807" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="E807" t="s">
         <v>86</v>
       </c>
       <c r="G807" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="808" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="808" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A808" t="s">
         <v>1014</v>
       </c>
       <c r="B808" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="C808" t="s">
-        <v>1001</v>
+        <v>1096</v>
       </c>
       <c r="D808" t="s">
-        <v>10</v>
-      </c>
-      <c r="G808" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="809" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1101</v>
+      </c>
+      <c r="E808" t="s">
+        <v>86</v>
+      </c>
+      <c r="G808" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="809" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A809" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B809" t="s">
-        <v>1037</v>
+        <v>1029</v>
       </c>
       <c r="C809" t="s">
-        <v>1001</v>
+        <v>1097</v>
       </c>
       <c r="D809" t="s">
-        <v>10</v>
-      </c>
-      <c r="G809" s="3">
-        <v>1</v>
+        <v>1102</v>
+      </c>
+      <c r="E809" t="s">
+        <v>86</v>
+      </c>
+      <c r="G809" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="810" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A810" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B810" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C810" t="s">
         <v>1001</v>
@@ -19995,50 +20004,50 @@
     </row>
     <row r="811" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A811" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B811" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
       <c r="C811" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D811" t="s">
-        <v>1016</v>
+        <v>10</v>
       </c>
       <c r="G811" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="812" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A812" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B812" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="C812" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D812" t="s">
-        <v>1016</v>
+        <v>10</v>
       </c>
       <c r="G812" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="813" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A813" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B813" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="C813" t="s">
         <v>1002</v>
       </c>
       <c r="D813" t="s">
-        <v>1039</v>
+        <v>1016</v>
       </c>
       <c r="G813" s="3">
         <v>2</v>
@@ -20046,19 +20055,16 @@
     </row>
     <row r="814" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A814" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B814" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C814" t="s">
         <v>1002</v>
       </c>
       <c r="D814" t="s">
-        <v>1039</v>
-      </c>
-      <c r="E814" t="s">
-        <v>86</v>
+        <v>1016</v>
       </c>
       <c r="G814" s="3">
         <v>2</v>
@@ -20066,42 +20072,36 @@
     </row>
     <row r="815" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A815" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B815" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
       <c r="C815" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D815" t="s">
-        <v>1017</v>
-      </c>
-      <c r="E815" t="s">
-        <v>86</v>
+        <v>1039</v>
       </c>
       <c r="G815" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="816" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A816" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B816" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="C816" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D816" t="s">
-        <v>1017</v>
-      </c>
-      <c r="E816" t="s">
-        <v>86</v>
+        <v>1039</v>
       </c>
       <c r="G816" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="817" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20112,16 +20112,16 @@
         <v>1034</v>
       </c>
       <c r="C817" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D817" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E817" t="s">
         <v>86</v>
       </c>
       <c r="G817" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="818" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20132,213 +20132,189 @@
         <v>1035</v>
       </c>
       <c r="C818" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D818" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E818" t="s">
         <v>86</v>
       </c>
       <c r="G818" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="819" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A819" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B819" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="C819" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D819" t="s">
-        <v>1040</v>
+        <v>1018</v>
       </c>
       <c r="E819" t="s">
         <v>86</v>
       </c>
       <c r="G819" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="820" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A820" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B820" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C820" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D820" t="s">
-        <v>1040</v>
+        <v>1018</v>
       </c>
       <c r="E820" t="s">
         <v>86</v>
       </c>
       <c r="G820" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="821" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A821" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B821" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C821" t="s">
-        <v>1006</v>
+        <v>1112</v>
       </c>
       <c r="D821" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E821" t="s">
-        <v>86</v>
+        <v>1113</v>
       </c>
       <c r="G821" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="822" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A822" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B822" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C822" t="s">
-        <v>1006</v>
+        <v>1112</v>
       </c>
       <c r="D822" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E822" t="s">
-        <v>86</v>
+        <v>1113</v>
       </c>
       <c r="G822" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="823" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A823" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B823" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="C823" t="s">
-        <v>1019</v>
+        <v>1004</v>
       </c>
       <c r="D823" t="s">
-        <v>1042</v>
-      </c>
-      <c r="E823" t="s">
-        <v>86</v>
+        <v>1040</v>
       </c>
       <c r="G823" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="824" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A824" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B824" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="C824" t="s">
-        <v>1021</v>
+        <v>1004</v>
       </c>
       <c r="D824" t="s">
-        <v>1043</v>
-      </c>
-      <c r="E824" t="s">
-        <v>86</v>
+        <v>1040</v>
       </c>
       <c r="G824" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="825" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A825" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B825" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="C825" t="s">
-        <v>1023</v>
+        <v>1006</v>
       </c>
       <c r="D825" t="s">
-        <v>1044</v>
-      </c>
-      <c r="E825" t="s">
-        <v>86</v>
+        <v>1041</v>
       </c>
       <c r="G825" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="826" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A826" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B826" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="C826" t="s">
-        <v>1027</v>
+        <v>1006</v>
       </c>
       <c r="D826" t="s">
-        <v>1045</v>
-      </c>
-      <c r="E826" t="s">
-        <v>86</v>
+        <v>1041</v>
       </c>
       <c r="G826" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="827" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A827" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B827" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="C827" t="s">
-        <v>1025</v>
+        <v>1112</v>
       </c>
       <c r="D827" t="s">
-        <v>1046</v>
-      </c>
-      <c r="E827" t="s">
-        <v>86</v>
+        <v>1114</v>
       </c>
       <c r="G827" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="828" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A828" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B828" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
       <c r="C828" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="D828" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E828" t="s">
-        <v>86</v>
+        <v>1114</v>
       </c>
       <c r="G828" s="3">
         <v>5</v>
@@ -20349,13 +20325,13 @@
         <v>1014</v>
       </c>
       <c r="B829" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C829" t="s">
-        <v>1030</v>
+        <v>1019</v>
       </c>
       <c r="D829" t="s">
-        <v>1047</v>
+        <v>1042</v>
       </c>
       <c r="E829" t="s">
         <v>86</v>
@@ -20369,13 +20345,13 @@
         <v>1014</v>
       </c>
       <c r="B830" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C830" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
       <c r="D830" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
       <c r="E830" t="s">
         <v>86</v>
@@ -20389,13 +20365,13 @@
         <v>1014</v>
       </c>
       <c r="B831" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C831" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D831" t="s">
-        <v>1049</v>
+        <v>1044</v>
       </c>
       <c r="E831" t="s">
         <v>86</v>
@@ -20404,47 +20380,47 @@
         <v>8</v>
       </c>
     </row>
-    <row r="832" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="832" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A832" t="s">
         <v>1014</v>
       </c>
       <c r="B832" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C832" t="s">
-        <v>1093</v>
+        <v>1027</v>
       </c>
       <c r="D832" t="s">
-        <v>1103</v>
+        <v>1045</v>
       </c>
       <c r="E832" t="s">
         <v>86</v>
       </c>
-      <c r="G832" s="2">
+      <c r="G832" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="833" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="833" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A833" t="s">
         <v>1014</v>
       </c>
       <c r="B833" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C833" t="s">
-        <v>1094</v>
+        <v>1025</v>
       </c>
       <c r="D833" t="s">
-        <v>1104</v>
+        <v>1046</v>
       </c>
       <c r="E833" t="s">
         <v>86</v>
       </c>
-      <c r="G833" s="2">
+      <c r="G833" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="834" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="834" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A834" t="s">
         <v>1014</v>
       </c>
@@ -20452,19 +20428,19 @@
         <v>1034</v>
       </c>
       <c r="C834" t="s">
-        <v>1095</v>
+        <v>1108</v>
       </c>
       <c r="D834" t="s">
-        <v>1106</v>
+        <v>1092</v>
       </c>
       <c r="E834" t="s">
         <v>86</v>
       </c>
-      <c r="G834" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="835" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G834" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="835" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A835" t="s">
         <v>1014</v>
       </c>
@@ -20472,19 +20448,19 @@
         <v>1034</v>
       </c>
       <c r="C835" t="s">
-        <v>1096</v>
+        <v>1030</v>
       </c>
       <c r="D835" t="s">
-        <v>1105</v>
+        <v>1047</v>
       </c>
       <c r="E835" t="s">
         <v>86</v>
       </c>
-      <c r="G835" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="836" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G835" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="836" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A836" t="s">
         <v>1014</v>
       </c>
@@ -20492,136 +20468,136 @@
         <v>1034</v>
       </c>
       <c r="C836" t="s">
-        <v>1097</v>
+        <v>1027</v>
       </c>
       <c r="D836" t="s">
-        <v>1107</v>
+        <v>1048</v>
       </c>
       <c r="E836" t="s">
         <v>86</v>
       </c>
-      <c r="G836" s="2">
-        <v>13</v>
+      <c r="G836" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="837" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A837" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B837" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C837" t="s">
-        <v>1050</v>
+        <v>1025</v>
       </c>
       <c r="D837" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="E837" t="s">
         <v>86</v>
       </c>
       <c r="G837" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="838" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="838" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A838" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B838" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C838" t="s">
-        <v>1052</v>
+        <v>1093</v>
       </c>
       <c r="D838" t="s">
-        <v>1053</v>
+        <v>1103</v>
       </c>
       <c r="E838" t="s">
         <v>86</v>
       </c>
-      <c r="G838" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="839" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G838" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="839" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A839" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B839" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C839" t="s">
-        <v>1054</v>
+        <v>1094</v>
       </c>
       <c r="D839" t="s">
-        <v>1055</v>
+        <v>1104</v>
       </c>
       <c r="E839" t="s">
         <v>86</v>
       </c>
-      <c r="G839" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="840" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G839" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="840" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A840" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B840" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C840" t="s">
-        <v>1056</v>
+        <v>1095</v>
       </c>
       <c r="D840" t="s">
-        <v>1057</v>
+        <v>1106</v>
       </c>
       <c r="E840" t="s">
         <v>86</v>
       </c>
-      <c r="G840" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="841" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G840" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="841" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A841" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B841" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C841" t="s">
-        <v>1058</v>
+        <v>1096</v>
       </c>
       <c r="D841" t="s">
-        <v>1059</v>
+        <v>1105</v>
       </c>
       <c r="E841" t="s">
         <v>86</v>
       </c>
-      <c r="G841" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="842" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G841" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="842" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A842" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="B842" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C842" t="s">
-        <v>1060</v>
+        <v>1097</v>
       </c>
       <c r="D842" t="s">
-        <v>1061</v>
+        <v>1107</v>
       </c>
       <c r="E842" t="s">
         <v>86</v>
       </c>
-      <c r="G842" s="3">
-        <v>10</v>
+      <c r="G842" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="843" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20632,16 +20608,16 @@
         <v>1038</v>
       </c>
       <c r="C843" t="s">
-        <v>1062</v>
+        <v>1050</v>
       </c>
       <c r="D843" t="s">
-        <v>1063</v>
+        <v>1051</v>
       </c>
       <c r="E843" t="s">
         <v>86</v>
       </c>
       <c r="G843" s="3">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="844" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20652,16 +20628,16 @@
         <v>1038</v>
       </c>
       <c r="C844" t="s">
-        <v>1064</v>
+        <v>1052</v>
       </c>
       <c r="D844" t="s">
-        <v>1065</v>
+        <v>1053</v>
       </c>
       <c r="E844" t="s">
         <v>86</v>
       </c>
       <c r="G844" s="3">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="845" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20672,16 +20648,16 @@
         <v>1038</v>
       </c>
       <c r="C845" t="s">
-        <v>1066</v>
+        <v>1054</v>
       </c>
       <c r="D845" t="s">
-        <v>1067</v>
+        <v>1055</v>
       </c>
       <c r="E845" t="s">
         <v>86</v>
       </c>
       <c r="G845" s="3">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="846" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20692,16 +20668,16 @@
         <v>1038</v>
       </c>
       <c r="C846" t="s">
-        <v>1068</v>
+        <v>1056</v>
       </c>
       <c r="D846" t="s">
-        <v>1069</v>
+        <v>1057</v>
       </c>
       <c r="E846" t="s">
         <v>86</v>
       </c>
       <c r="G846" s="3">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="847" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20712,16 +20688,16 @@
         <v>1038</v>
       </c>
       <c r="C847" t="s">
-        <v>1070</v>
+        <v>1058</v>
       </c>
       <c r="D847" t="s">
-        <v>1071</v>
+        <v>1059</v>
       </c>
       <c r="E847" t="s">
         <v>86</v>
       </c>
       <c r="G847" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="848" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20732,16 +20708,16 @@
         <v>1038</v>
       </c>
       <c r="C848" t="s">
-        <v>1072</v>
+        <v>1060</v>
       </c>
       <c r="D848" t="s">
-        <v>1073</v>
+        <v>1061</v>
       </c>
       <c r="E848" t="s">
         <v>86</v>
       </c>
       <c r="G848" s="3">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="849" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20752,16 +20728,16 @@
         <v>1038</v>
       </c>
       <c r="C849" t="s">
-        <v>1074</v>
+        <v>1062</v>
       </c>
       <c r="D849" t="s">
-        <v>1075</v>
+        <v>1063</v>
       </c>
       <c r="E849" t="s">
         <v>86</v>
       </c>
       <c r="G849" s="3">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="850" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20769,19 +20745,19 @@
         <v>1036</v>
       </c>
       <c r="B850" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C850" t="s">
-        <v>1019</v>
+        <v>1064</v>
       </c>
       <c r="D850" t="s">
-        <v>1076</v>
+        <v>1065</v>
       </c>
       <c r="E850" t="s">
         <v>86</v>
       </c>
       <c r="G850" s="3">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="851" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20789,19 +20765,19 @@
         <v>1036</v>
       </c>
       <c r="B851" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C851" t="s">
-        <v>1077</v>
+        <v>1066</v>
       </c>
       <c r="D851" t="s">
-        <v>1078</v>
+        <v>1067</v>
       </c>
       <c r="E851" t="s">
         <v>86</v>
       </c>
       <c r="G851" s="3">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="852" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20809,19 +20785,19 @@
         <v>1036</v>
       </c>
       <c r="B852" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C852" t="s">
-        <v>1079</v>
+        <v>1068</v>
       </c>
       <c r="D852" t="s">
-        <v>1080</v>
+        <v>1069</v>
       </c>
       <c r="E852" t="s">
         <v>86</v>
       </c>
       <c r="G852" s="3">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="853" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20829,19 +20805,19 @@
         <v>1036</v>
       </c>
       <c r="B853" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C853" t="s">
-        <v>1081</v>
+        <v>1070</v>
       </c>
       <c r="D853" t="s">
-        <v>1082</v>
+        <v>1071</v>
       </c>
       <c r="E853" t="s">
         <v>86</v>
       </c>
       <c r="G853" s="3">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="854" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20849,19 +20825,19 @@
         <v>1036</v>
       </c>
       <c r="B854" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C854" t="s">
-        <v>1083</v>
+        <v>1072</v>
       </c>
       <c r="D854" t="s">
-        <v>1084</v>
+        <v>1073</v>
       </c>
       <c r="E854" t="s">
         <v>86</v>
       </c>
       <c r="G854" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="855" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20869,19 +20845,19 @@
         <v>1036</v>
       </c>
       <c r="B855" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C855" t="s">
-        <v>1085</v>
+        <v>1074</v>
       </c>
       <c r="D855" t="s">
-        <v>1086</v>
+        <v>1075</v>
       </c>
       <c r="E855" t="s">
         <v>86</v>
       </c>
       <c r="G855" s="3">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="856" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20892,16 +20868,16 @@
         <v>1037</v>
       </c>
       <c r="C856" t="s">
-        <v>1087</v>
+        <v>1019</v>
       </c>
       <c r="D856" t="s">
-        <v>1088</v>
+        <v>1076</v>
       </c>
       <c r="E856" t="s">
         <v>86</v>
       </c>
       <c r="G856" s="3">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="857" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20912,16 +20888,16 @@
         <v>1037</v>
       </c>
       <c r="C857" t="s">
-        <v>1072</v>
+        <v>1077</v>
       </c>
       <c r="D857" t="s">
-        <v>1089</v>
+        <v>1078</v>
       </c>
       <c r="E857" t="s">
         <v>86</v>
       </c>
       <c r="G857" s="3">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="858" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -20932,54 +20908,174 @@
         <v>1037</v>
       </c>
       <c r="C858" t="s">
-        <v>1074</v>
+        <v>1079</v>
       </c>
       <c r="D858" t="s">
-        <v>1090</v>
+        <v>1080</v>
       </c>
       <c r="E858" t="s">
         <v>86</v>
       </c>
       <c r="G858" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="859" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A859" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B859" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C859" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D859" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E859" t="s">
+        <v>86</v>
+      </c>
+      <c r="G859" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="860" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A860" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B860" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C860" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D860" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E860" t="s">
+        <v>86</v>
+      </c>
+      <c r="G860" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="861" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A861" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B861" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C861" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D861" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E861" t="s">
+        <v>86</v>
+      </c>
+      <c r="G861" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="862" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A862" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B862" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C862" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D862" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E862" t="s">
+        <v>86</v>
+      </c>
+      <c r="G862" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="863" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A863" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B863" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C863" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D863" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E863" t="s">
+        <v>86</v>
+      </c>
+      <c r="G863" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="859" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A859" t="s">
+    <row r="864" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A864" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B864" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C864" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D864" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E864" t="s">
+        <v>86</v>
+      </c>
+      <c r="G864" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="865" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A865" t="s">
         <v>1014</v>
       </c>
-      <c r="B859" t="s">
+      <c r="B865" t="s">
         <v>1109</v>
       </c>
-      <c r="C859" t="s">
+      <c r="C865" t="s">
         <v>1001</v>
       </c>
-      <c r="D859" t="s">
+      <c r="D865" t="s">
         <v>10</v>
       </c>
-      <c r="G859" s="2">
+      <c r="G865" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="860" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A860" t="s">
+    <row r="866" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A866" t="s">
         <v>1014</v>
       </c>
-      <c r="B860" t="s">
+      <c r="B866" t="s">
         <v>1109</v>
       </c>
-      <c r="C860" t="s">
+      <c r="C866" t="s">
         <v>1110</v>
       </c>
-      <c r="D860" t="s">
+      <c r="D866" t="s">
         <v>1111</v>
       </c>
-      <c r="G860" s="2">
+      <c r="G866" s="2">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H858" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H866" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>